<commit_message>
added TaskValidator + updated Controller, NewEditController, TasksService
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27504"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7FEDABB8-B8B1-4D7F-B374-801E6280C83E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3AA89D67-13F3-4512-8938-C3203D6F2471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="156" windowWidth="14160" windowHeight="8268" tabRatio="650" firstSheet="3" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="156" windowWidth="14160" windowHeight="8268" tabRatio="650" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="70">
   <si>
     <t>do not print this form</t>
   </si>
@@ -189,7 +189,13 @@
     <t>Task</t>
   </si>
   <si>
-    <t>(DA) Entitatea aplicatiei (Task) expune functionalitatile si operatiile necesare aplicatiei.</t>
+    <t xml:space="preserve">(DA) Entitatea aplicatiei (Task) nu expune functionalitatile si operatiile necesare aplicatiei. Nu ar trebui sa avem validari in constructorul clasei Task. </t>
+  </si>
+  <si>
+    <t>TasksService</t>
+  </si>
+  <si>
+    <t>Nu exisa validari pe backend =&gt; avem nevoie de validator in service</t>
   </si>
   <si>
     <t>Review Form. Coding Defects</t>
@@ -199,6 +205,24 @@
   </si>
   <si>
     <t>Popescu Ionel</t>
+  </si>
+  <si>
+    <t>C09</t>
+  </si>
+  <si>
+    <t>Main</t>
+  </si>
+  <si>
+    <t>Cod duplicat: TasksService se creeaza de 2 ori in Main</t>
+  </si>
+  <si>
+    <t>Cod nefolosit: classLoader din Main</t>
+  </si>
+  <si>
+    <t>Controller</t>
+  </si>
+  <si>
+    <t>mainTable este o copie statica a tabelului tasks =&gt; nu avem nevoie de ea, putem lucra direct cu tasks</t>
   </si>
   <si>
     <t>Tool-based Code Analysis</t>
@@ -414,8 +438,15 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -430,6 +461,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -452,16 +486,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -798,27 +822,27 @@
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
       <c r="G1" s="16"/>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="16"/>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32" t="s">
+      <c r="H2" s="17"/>
+      <c r="I2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="J2" s="17" t="s">
         <v>4</v>
       </c>
     </row>
@@ -830,11 +854,11 @@
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
-      <c r="H3" s="32" t="s">
+      <c r="H3" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="16"/>
@@ -842,17 +866,17 @@
       <c r="C4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="19"/>
+      <c r="E4" s="22"/>
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
-      <c r="H4" s="32" t="s">
+      <c r="H4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="16"/>
@@ -860,17 +884,17 @@
       <c r="C5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="21"/>
+      <c r="E5" s="24"/>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
-      <c r="H5" s="32" t="s">
+      <c r="H5" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="16"/>
@@ -878,8 +902,8 @@
       <c r="C6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
       <c r="H6" s="16"/>
@@ -892,8 +916,8 @@
       <c r="C7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
       <c r="H7" s="16"/>
@@ -922,7 +946,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="16"/>
-      <c r="B10" s="32">
+      <c r="B10" s="17">
         <v>1</v>
       </c>
       <c r="C10" s="1"/>
@@ -936,7 +960,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="16"/>
-      <c r="B11" s="32">
+      <c r="B11" s="17">
         <f>B10+1</f>
         <v>2</v>
       </c>
@@ -951,7 +975,7 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="16"/>
-      <c r="B12" s="32">
+      <c r="B12" s="17">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
       </c>
@@ -966,7 +990,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="16"/>
-      <c r="B13" s="32">
+      <c r="B13" s="17">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -981,7 +1005,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="16"/>
-      <c r="B14" s="32">
+      <c r="B14" s="17">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -996,7 +1020,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="16"/>
-      <c r="B15" s="32">
+      <c r="B15" s="17">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -1011,7 +1035,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="16"/>
-      <c r="B16" s="32">
+      <c r="B16" s="17">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
@@ -1025,7 +1049,7 @@
       <c r="J16" s="16"/>
     </row>
     <row r="17" spans="2:5">
-      <c r="B17" s="32">
+      <c r="B17" s="17">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
@@ -1034,76 +1058,76 @@
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="2:5">
-      <c r="B18" s="32">
+      <c r="B18" s="17">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="33"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="18"/>
     </row>
     <row r="19" spans="2:5">
-      <c r="B19" s="32">
+      <c r="B19" s="17">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C19" s="32"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="33"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="18"/>
     </row>
     <row r="20" spans="2:5">
-      <c r="B20" s="32">
+      <c r="B20" s="17">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="33"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="18"/>
     </row>
     <row r="21" spans="2:5">
-      <c r="B21" s="32">
+      <c r="B21" s="17">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C21" s="32"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="33"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="18"/>
     </row>
     <row r="22" spans="2:5">
-      <c r="B22" s="32">
+      <c r="B22" s="17">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="33"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="18"/>
     </row>
     <row r="23" spans="2:5">
-      <c r="B23" s="32">
+      <c r="B23" s="17">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C23" s="32"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="33"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="18"/>
     </row>
     <row r="24" spans="2:5">
-      <c r="B24" s="32">
+      <c r="B24" s="17">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C24" s="32"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="33"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="18"/>
     </row>
     <row r="25" spans="2:5">
-      <c r="B25" s="32">
+      <c r="B25" s="17">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C25" s="32"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="33"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="18"/>
     </row>
     <row r="26" spans="2:5">
       <c r="B26" s="16"/>
@@ -1140,8 +1164,8 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:E7"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
@@ -1165,27 +1189,27 @@
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
       <c r="G1" s="16"/>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="16"/>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32" t="s">
+      <c r="H2" s="17"/>
+      <c r="I2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="J2" s="17" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1197,13 +1221,13 @@
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
-      <c r="H3" s="32" t="s">
+      <c r="H3" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="32" t="s">
+      <c r="I3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="32">
+      <c r="J3" s="17">
         <v>233</v>
       </c>
     </row>
@@ -1213,19 +1237,19 @@
       <c r="C4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="22"/>
+      <c r="E4" s="25"/>
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
-      <c r="H4" s="32" t="s">
+      <c r="H4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="32" t="s">
+      <c r="I4" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="32">
+      <c r="J4" s="17">
         <v>231</v>
       </c>
     </row>
@@ -1235,19 +1259,19 @@
       <c r="C5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="24"/>
+      <c r="E5" s="28"/>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
-      <c r="H5" s="32" t="s">
+      <c r="H5" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="32" t="s">
+      <c r="I5" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="J5" s="32">
+      <c r="J5" s="17">
         <v>231</v>
       </c>
     </row>
@@ -1257,10 +1281,10 @@
       <c r="C6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="17"/>
+      <c r="E6" s="19"/>
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
       <c r="H6" s="16"/>
@@ -1273,10 +1297,10 @@
       <c r="C7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="30">
+      <c r="D7" s="26">
         <v>45361</v>
       </c>
-      <c r="E7" s="17"/>
+      <c r="E7" s="19"/>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
       <c r="H7" s="16"/>
@@ -1305,7 +1329,7 @@
     </row>
     <row r="10" spans="1:10" ht="60.75">
       <c r="A10" s="16"/>
-      <c r="B10" s="32">
+      <c r="B10" s="17">
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1325,7 +1349,7 @@
     </row>
     <row r="11" spans="1:10" ht="106.5">
       <c r="A11" s="16"/>
-      <c r="B11" s="32">
+      <c r="B11" s="17">
         <f>B10+1</f>
         <v>2</v>
       </c>
@@ -1346,7 +1370,7 @@
     </row>
     <row r="12" spans="1:10" ht="45.75">
       <c r="A12" s="16"/>
-      <c r="B12" s="32">
+      <c r="B12" s="17">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
       </c>
@@ -1365,7 +1389,7 @@
     </row>
     <row r="13" spans="1:10" ht="106.5">
       <c r="A13" s="16"/>
-      <c r="B13" s="32">
+      <c r="B13" s="17">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -1386,7 +1410,7 @@
     </row>
     <row r="14" spans="1:10" ht="183">
       <c r="A14" s="16"/>
-      <c r="B14" s="32">
+      <c r="B14" s="17">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -1407,7 +1431,7 @@
     </row>
     <row r="15" spans="1:10" ht="45.75">
       <c r="A15" s="16"/>
-      <c r="B15" s="32">
+      <c r="B15" s="17">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -1428,7 +1452,7 @@
     </row>
     <row r="16" spans="1:10" ht="76.5">
       <c r="A16" s="16"/>
-      <c r="B16" s="32">
+      <c r="B16" s="17">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
@@ -1448,7 +1472,7 @@
       <c r="J16" s="16"/>
     </row>
     <row r="17" spans="2:5" ht="60.75">
-      <c r="B17" s="32">
+      <c r="B17" s="17">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
@@ -1462,8 +1486,8 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="45.75">
-      <c r="B18" s="32">
+    <row r="18" spans="2:5" ht="60.75">
+      <c r="B18" s="17">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
@@ -1477,17 +1501,23 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="2:5">
-      <c r="B19" s="32">
+    <row r="19" spans="2:5" ht="30.75">
+      <c r="B19" s="17">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="C19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="20" spans="2:5">
-      <c r="B20" s="32">
+      <c r="B20" s="17">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
@@ -1496,7 +1526,7 @@
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="2:5">
-      <c r="B21" s="32">
+      <c r="B21" s="17">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -1505,7 +1535,7 @@
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="2:5">
-      <c r="B22" s="32">
+      <c r="B22" s="17">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
@@ -1514,7 +1544,7 @@
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="2:5">
-      <c r="B23" s="32">
+      <c r="B23" s="17">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
@@ -1523,7 +1553,7 @@
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="2:5">
-      <c r="B24" s="32">
+      <c r="B24" s="17">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -1532,7 +1562,7 @@
       <c r="E24" s="2"/>
     </row>
     <row r="25" spans="2:5">
-      <c r="B25" s="32">
+      <c r="B25" s="17">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
@@ -1541,7 +1571,7 @@
       <c r="E25" s="2"/>
     </row>
     <row r="26" spans="2:5">
-      <c r="B26" s="32">
+      <c r="B26" s="17">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
@@ -1584,8 +1614,8 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
@@ -1610,27 +1640,27 @@
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
       <c r="G1" s="16"/>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="16"/>
-      <c r="B2" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
+      <c r="B2" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32" t="s">
+      <c r="H2" s="17"/>
+      <c r="I2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="J2" s="17" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1642,11 +1672,11 @@
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
-      <c r="H3" s="32" t="s">
+      <c r="H3" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="16"/>
@@ -1654,17 +1684,17 @@
       <c r="C4" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="E4" s="25"/>
+      <c r="D4" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="29"/>
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
-      <c r="H4" s="32" t="s">
+      <c r="H4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="16"/>
@@ -1672,17 +1702,17 @@
       <c r="C5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="E5" s="27"/>
+      <c r="D5" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="31"/>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
-      <c r="H5" s="32" t="s">
+      <c r="H5" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="16"/>
@@ -1690,8 +1720,8 @@
       <c r="C6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
       <c r="H6" s="16"/>
@@ -1704,8 +1734,8 @@
       <c r="C7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
       <c r="H7" s="16"/>
@@ -1732,44 +1762,62 @@
       <c r="I9" s="16"/>
       <c r="J9" s="16"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" ht="30.75">
       <c r="A10" s="16"/>
-      <c r="B10" s="32">
+      <c r="B10" s="17">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="C10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
       <c r="H10" s="16"/>
       <c r="I10" s="16"/>
       <c r="J10" s="16"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" ht="15">
       <c r="A11" s="16"/>
-      <c r="B11" s="32">
+      <c r="B11" s="17">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
+      <c r="C11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
       <c r="H11" s="16"/>
       <c r="I11" s="16"/>
       <c r="J11" s="16"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" ht="45.75">
       <c r="A12" s="16"/>
-      <c r="B12" s="32">
+      <c r="B12" s="17">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
+      <c r="C12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
       <c r="H12" s="16"/>
@@ -1778,7 +1826,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="16"/>
-      <c r="B13" s="32">
+      <c r="B13" s="17">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -1793,7 +1841,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="16"/>
-      <c r="B14" s="32">
+      <c r="B14" s="17">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -1808,7 +1856,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="16"/>
-      <c r="B15" s="32">
+      <c r="B15" s="17">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -1823,7 +1871,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="16"/>
-      <c r="B16" s="32">
+      <c r="B16" s="17">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
@@ -1837,7 +1885,7 @@
       <c r="J16" s="16"/>
     </row>
     <row r="17" spans="2:5">
-      <c r="B17" s="32">
+      <c r="B17" s="17">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
@@ -1846,7 +1894,7 @@
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="2:5">
-      <c r="B18" s="32">
+      <c r="B18" s="17">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
@@ -1855,7 +1903,7 @@
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="2:5">
-      <c r="B19" s="32">
+      <c r="B19" s="17">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
@@ -1864,7 +1912,7 @@
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="2:5">
-      <c r="B20" s="32">
+      <c r="B20" s="17">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
@@ -1873,7 +1921,7 @@
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="2:5">
-      <c r="B21" s="32">
+      <c r="B21" s="17">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -1882,7 +1930,7 @@
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="2:5">
-      <c r="B22" s="32">
+      <c r="B22" s="17">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
@@ -1891,7 +1939,7 @@
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="2:5">
-      <c r="B23" s="32">
+      <c r="B23" s="17">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
@@ -1900,7 +1948,7 @@
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="2:5">
-      <c r="B24" s="32">
+      <c r="B24" s="17">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -1909,7 +1957,7 @@
       <c r="E24" s="2"/>
     </row>
     <row r="25" spans="2:5">
-      <c r="B25" s="32">
+      <c r="B25" s="17">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
@@ -1918,7 +1966,7 @@
       <c r="E25" s="2"/>
     </row>
     <row r="26" spans="2:5">
-      <c r="B26" s="32">
+      <c r="B26" s="17">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
@@ -1927,7 +1975,7 @@
       <c r="E26" s="2"/>
     </row>
     <row r="27" spans="2:5">
-      <c r="B27" s="32">
+      <c r="B27" s="17">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
@@ -1936,7 +1984,7 @@
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="2:5">
-      <c r="B28" s="32">
+      <c r="B28" s="17">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
@@ -1945,7 +1993,7 @@
       <c r="E28" s="2"/>
     </row>
     <row r="29" spans="2:5">
-      <c r="B29" s="32">
+      <c r="B29" s="17">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
@@ -1954,7 +2002,7 @@
       <c r="E29" s="2"/>
     </row>
     <row r="30" spans="2:5">
-      <c r="B30" s="32">
+      <c r="B30" s="17">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
@@ -2024,27 +2072,27 @@
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
       <c r="G1" s="16"/>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="16"/>
-      <c r="B2" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
+      <c r="B2" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32" t="s">
+      <c r="H2" s="17"/>
+      <c r="I2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="J2" s="17" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2056,27 +2104,27 @@
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
-      <c r="H3" s="32" t="s">
+      <c r="H3" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="16"/>
       <c r="B4" s="16"/>
       <c r="C4" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
+        <v>64</v>
+      </c>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
-      <c r="H4" s="32" t="s">
+      <c r="H4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="16"/>
@@ -2084,15 +2132,15 @@
       <c r="C5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
-      <c r="H5" s="32" t="s">
+      <c r="H5" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="16"/>
@@ -2100,8 +2148,8 @@
       <c r="C6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
       <c r="H6" s="16"/>
@@ -2114,16 +2162,16 @@
         <v>14</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="G9" s="16"/>
       <c r="H9" s="16"/>
@@ -2132,7 +2180,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="16"/>
-      <c r="B10" s="32">
+      <c r="B10" s="17">
         <v>1</v>
       </c>
       <c r="C10" s="1"/>
@@ -2146,7 +2194,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="16"/>
-      <c r="B11" s="32">
+      <c r="B11" s="17">
         <f>B10+1</f>
         <v>2</v>
       </c>
@@ -2161,7 +2209,7 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="16"/>
-      <c r="B12" s="32">
+      <c r="B12" s="17">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
@@ -2176,7 +2224,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="16"/>
-      <c r="B13" s="32">
+      <c r="B13" s="17">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -2191,7 +2239,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="16"/>
-      <c r="B14" s="32">
+      <c r="B14" s="17">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -2206,7 +2254,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="16"/>
-      <c r="B15" s="32">
+      <c r="B15" s="17">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -2221,7 +2269,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="16"/>
-      <c r="B16" s="32">
+      <c r="B16" s="17">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
@@ -2235,7 +2283,7 @@
       <c r="J16" s="16"/>
     </row>
     <row r="17" spans="2:6">
-      <c r="B17" s="32">
+      <c r="B17" s="17">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
@@ -2245,7 +2293,7 @@
       <c r="F17" s="2"/>
     </row>
     <row r="18" spans="2:6">
-      <c r="B18" s="32">
+      <c r="B18" s="17">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
@@ -2255,7 +2303,7 @@
       <c r="F18" s="2"/>
     </row>
     <row r="19" spans="2:6">
-      <c r="B19" s="32">
+      <c r="B19" s="17">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
@@ -2265,7 +2313,7 @@
       <c r="F19" s="2"/>
     </row>
     <row r="20" spans="2:6">
-      <c r="B20" s="32">
+      <c r="B20" s="17">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
@@ -2275,7 +2323,7 @@
       <c r="F20" s="2"/>
     </row>
     <row r="21" spans="2:6">
-      <c r="B21" s="32">
+      <c r="B21" s="17">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -2285,7 +2333,7 @@
       <c r="F21" s="2"/>
     </row>
     <row r="22" spans="2:6">
-      <c r="B22" s="32">
+      <c r="B22" s="17">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
@@ -2295,7 +2343,7 @@
       <c r="F22" s="2"/>
     </row>
     <row r="23" spans="2:6">
-      <c r="B23" s="32">
+      <c r="B23" s="17">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
@@ -2305,7 +2353,7 @@
       <c r="F23" s="2"/>
     </row>
     <row r="24" spans="2:6">
-      <c r="B24" s="32">
+      <c r="B24" s="17">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -2315,7 +2363,7 @@
       <c r="F24" s="2"/>
     </row>
     <row r="25" spans="2:6">
-      <c r="B25" s="32">
+      <c r="B25" s="17">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
@@ -2325,7 +2373,7 @@
       <c r="F25" s="2"/>
     </row>
     <row r="26" spans="2:6">
-      <c r="B26" s="32">
+      <c r="B26" s="17">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
@@ -2335,7 +2383,7 @@
       <c r="F26" s="2"/>
     </row>
     <row r="27" spans="2:6">
-      <c r="B27" s="32">
+      <c r="B27" s="17">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
@@ -2345,7 +2393,7 @@
       <c r="F27" s="1"/>
     </row>
     <row r="28" spans="2:6">
-      <c r="B28" s="32">
+      <c r="B28" s="17">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
@@ -2355,7 +2403,7 @@
       <c r="F28" s="2"/>
     </row>
     <row r="29" spans="2:6">
-      <c r="B29" s="32">
+      <c r="B29" s="17">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
@@ -2365,7 +2413,7 @@
       <c r="F29" s="2"/>
     </row>
     <row r="30" spans="2:6">
-      <c r="B30" s="32">
+      <c r="B30" s="17">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
@@ -2383,11 +2431,11 @@
     </row>
     <row r="32" spans="2:6">
       <c r="B32" s="16"/>
-      <c r="C32" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
+      <c r="C32" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33"/>
       <c r="F32" s="15"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 3 more arhitect. design
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27504"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3AA89D67-13F3-4512-8938-C3203D6F2471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\balut\Documents\Desktop_Folder\photoshop try\for learning(apps,etc)\ANUL III\VVSS\gitRepoLab\baxbaniiVVSS\Docs\Lab01\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{016B3A29-4878-4C3F-827F-3EE71DA0B20C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="156" windowWidth="14160" windowHeight="8268" tabRatio="650" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -25,8 +30,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="76">
   <si>
     <t>do not print this form</t>
   </si>
@@ -244,13 +247,31 @@
   </si>
   <si>
     <t>Effort to perform tool-based code analysis (hours):</t>
+  </si>
+  <si>
+    <t>A03/A04</t>
+  </si>
+  <si>
+    <t>Constructor does not match the requirements</t>
+  </si>
+  <si>
+    <t>Momery</t>
+  </si>
+  <si>
+    <t>No repo class to handle entity</t>
+  </si>
+  <si>
+    <t>TaskService</t>
+  </si>
+  <si>
+    <t>Service should not memorize entity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -505,9 +526,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -545,9 +566,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -580,9 +601,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -615,9 +653,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -796,11 +851,11 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="5"/>
     <col min="2" max="2" width="12.28515625" style="5" customWidth="1"/>
@@ -812,7 +867,7 @@
     <col min="11" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -828,7 +883,7 @@
       <c r="I1" s="20"/>
       <c r="J1" s="20"/>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="16"/>
       <c r="B2" s="21" t="s">
         <v>2</v>
@@ -846,7 +901,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="16"/>
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
@@ -860,7 +915,7 @@
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="16"/>
       <c r="B4" s="16"/>
       <c r="C4" s="12" t="s">
@@ -878,7 +933,7 @@
       <c r="I4" s="17"/>
       <c r="J4" s="17"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="B5" s="16"/>
       <c r="C5" s="12" t="s">
@@ -896,7 +951,7 @@
       <c r="I5" s="17"/>
       <c r="J5" s="17"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8" t="s">
@@ -910,7 +965,7 @@
       <c r="I6" s="16"/>
       <c r="J6" s="16"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
       <c r="B7" s="16"/>
       <c r="C7" s="8" t="s">
@@ -924,7 +979,7 @@
       <c r="I7" s="16"/>
       <c r="J7" s="16"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
       <c r="B9" s="9" t="s">
         <v>14</v>
@@ -944,7 +999,7 @@
       <c r="I9" s="16"/>
       <c r="J9" s="16"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="16"/>
       <c r="B10" s="17">
         <v>1</v>
@@ -958,7 +1013,7 @@
       <c r="I10" s="16"/>
       <c r="J10" s="16"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
       <c r="B11" s="17">
         <f>B10+1</f>
@@ -973,7 +1028,7 @@
       <c r="I11" s="16"/>
       <c r="J11" s="16"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="16"/>
       <c r="B12" s="17">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
@@ -988,7 +1043,7 @@
       <c r="I12" s="16"/>
       <c r="J12" s="16"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
       <c r="B13" s="17">
         <f t="shared" si="0"/>
@@ -1003,7 +1058,7 @@
       <c r="I13" s="16"/>
       <c r="J13" s="16"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="16"/>
       <c r="B14" s="17">
         <f t="shared" si="0"/>
@@ -1018,7 +1073,7 @@
       <c r="I14" s="16"/>
       <c r="J14" s="16"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="17">
         <f t="shared" si="0"/>
@@ -1033,7 +1088,7 @@
       <c r="I15" s="16"/>
       <c r="J15" s="16"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="16"/>
       <c r="B16" s="17">
         <f t="shared" si="0"/>
@@ -1048,7 +1103,7 @@
       <c r="I16" s="16"/>
       <c r="J16" s="16"/>
     </row>
-    <row r="17" spans="2:5">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="17">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1057,7 +1112,7 @@
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="17">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1066,7 +1121,7 @@
       <c r="D18" s="17"/>
       <c r="E18" s="18"/>
     </row>
-    <row r="19" spans="2:5">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="17">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1075,7 +1130,7 @@
       <c r="D19" s="17"/>
       <c r="E19" s="18"/>
     </row>
-    <row r="20" spans="2:5">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="17">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1084,7 +1139,7 @@
       <c r="D20" s="17"/>
       <c r="E20" s="18"/>
     </row>
-    <row r="21" spans="2:5">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="17">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1093,7 +1148,7 @@
       <c r="D21" s="17"/>
       <c r="E21" s="18"/>
     </row>
-    <row r="22" spans="2:5">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="17">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1102,7 +1157,7 @@
       <c r="D22" s="17"/>
       <c r="E22" s="18"/>
     </row>
-    <row r="23" spans="2:5">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="17">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1111,7 +1166,7 @@
       <c r="D23" s="17"/>
       <c r="E23" s="18"/>
     </row>
-    <row r="24" spans="2:5">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="17">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1120,7 +1175,7 @@
       <c r="D24" s="17"/>
       <c r="E24" s="18"/>
     </row>
-    <row r="25" spans="2:5">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1129,13 +1184,13 @@
       <c r="D25" s="17"/>
       <c r="E25" s="18"/>
     </row>
-    <row r="26" spans="2:5">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
       <c r="E26" s="16"/>
     </row>
-    <row r="27" spans="2:5">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="16"/>
       <c r="C27" s="10" t="s">
         <v>18</v>
@@ -1165,10 +1220,10 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="C20" sqref="C20:E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="5"/>
     <col min="2" max="2" width="12.28515625" style="5" customWidth="1"/>
@@ -1179,7 +1234,7 @@
     <col min="10" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -1195,7 +1250,7 @@
       <c r="I1" s="20"/>
       <c r="J1" s="20"/>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="16"/>
       <c r="B2" s="21" t="s">
         <v>19</v>
@@ -1213,7 +1268,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="16"/>
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
@@ -1231,7 +1286,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="16"/>
       <c r="B4" s="16"/>
       <c r="C4" s="6" t="s">
@@ -1253,7 +1308,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="B5" s="16"/>
       <c r="C5" s="6" t="s">
@@ -1275,7 +1330,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8" t="s">
@@ -1291,7 +1346,7 @@
       <c r="I6" s="16"/>
       <c r="J6" s="16"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
       <c r="B7" s="16"/>
       <c r="C7" s="8" t="s">
@@ -1307,7 +1362,7 @@
       <c r="I7" s="16"/>
       <c r="J7" s="16"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
       <c r="B9" s="9" t="s">
         <v>14</v>
@@ -1327,7 +1382,7 @@
       <c r="I9" s="16"/>
       <c r="J9" s="16"/>
     </row>
-    <row r="10" spans="1:10" ht="60.75">
+    <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="16"/>
       <c r="B10" s="17">
         <v>1</v>
@@ -1347,7 +1402,7 @@
       <c r="I10" s="16"/>
       <c r="J10" s="16"/>
     </row>
-    <row r="11" spans="1:10" ht="106.5">
+    <row r="11" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
       <c r="B11" s="17">
         <f>B10+1</f>
@@ -1368,7 +1423,7 @@
       <c r="I11" s="16"/>
       <c r="J11" s="16"/>
     </row>
-    <row r="12" spans="1:10" ht="45.75">
+    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="16"/>
       <c r="B12" s="17">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
@@ -1387,7 +1442,7 @@
       <c r="I12" s="16"/>
       <c r="J12" s="16"/>
     </row>
-    <row r="13" spans="1:10" ht="106.5">
+    <row r="13" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
       <c r="B13" s="17">
         <f t="shared" si="0"/>
@@ -1408,7 +1463,7 @@
       <c r="I13" s="16"/>
       <c r="J13" s="16"/>
     </row>
-    <row r="14" spans="1:10" ht="183">
+    <row r="14" spans="1:10" ht="195" x14ac:dyDescent="0.25">
       <c r="A14" s="16"/>
       <c r="B14" s="17">
         <f t="shared" si="0"/>
@@ -1429,7 +1484,7 @@
       <c r="I14" s="16"/>
       <c r="J14" s="16"/>
     </row>
-    <row r="15" spans="1:10" ht="45.75">
+    <row r="15" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="17">
         <f t="shared" si="0"/>
@@ -1450,7 +1505,7 @@
       <c r="I15" s="16"/>
       <c r="J15" s="16"/>
     </row>
-    <row r="16" spans="1:10" ht="76.5">
+    <row r="16" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="16"/>
       <c r="B16" s="17">
         <f t="shared" si="0"/>
@@ -1471,7 +1526,7 @@
       <c r="I16" s="16"/>
       <c r="J16" s="16"/>
     </row>
-    <row r="17" spans="2:5" ht="60.75">
+    <row r="17" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B17" s="17">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1486,7 +1541,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="60.75">
+    <row r="18" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B18" s="17">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1501,7 +1556,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="30.75">
+    <row r="19" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="17">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1516,34 +1571,52 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="2:5">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="17">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="2:5">
+      <c r="C20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="17">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="2:5">
+      <c r="C21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="17">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="2:5">
+      <c r="C22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="17">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1552,7 +1625,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="17">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1561,7 +1634,7 @@
       <c r="D24" s="1"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1570,7 +1643,7 @@
       <c r="D25" s="1"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="17">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1579,13 +1652,13 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="16"/>
       <c r="C27" s="16"/>
       <c r="D27" s="16"/>
       <c r="E27" s="16"/>
     </row>
-    <row r="28" spans="2:5">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="16"/>
       <c r="C28" s="10" t="s">
         <v>18</v>
@@ -1614,11 +1687,11 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="5"/>
     <col min="2" max="2" width="12.28515625" style="5" customWidth="1"/>
@@ -1630,7 +1703,7 @@
     <col min="10" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -1646,7 +1719,7 @@
       <c r="I1" s="20"/>
       <c r="J1" s="20"/>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="16"/>
       <c r="B2" s="21" t="s">
         <v>54</v>
@@ -1664,7 +1737,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="16"/>
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
@@ -1678,7 +1751,7 @@
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="16"/>
       <c r="B4" s="16"/>
       <c r="C4" s="14" t="s">
@@ -1696,7 +1769,7 @@
       <c r="I4" s="17"/>
       <c r="J4" s="17"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="B5" s="16"/>
       <c r="C5" s="14" t="s">
@@ -1714,7 +1787,7 @@
       <c r="I5" s="17"/>
       <c r="J5" s="17"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8" t="s">
@@ -1728,7 +1801,7 @@
       <c r="I6" s="16"/>
       <c r="J6" s="16"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
       <c r="B7" s="16"/>
       <c r="C7" s="8" t="s">
@@ -1742,7 +1815,7 @@
       <c r="I7" s="16"/>
       <c r="J7" s="16"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
       <c r="B9" s="9" t="s">
         <v>14</v>
@@ -1762,7 +1835,7 @@
       <c r="I9" s="16"/>
       <c r="J9" s="16"/>
     </row>
-    <row r="10" spans="1:10" ht="30.75">
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="16"/>
       <c r="B10" s="17">
         <v>1</v>
@@ -1782,7 +1855,7 @@
       <c r="I10" s="16"/>
       <c r="J10" s="16"/>
     </row>
-    <row r="11" spans="1:10" ht="15">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
       <c r="B11" s="17">
         <f>B10+1</f>
@@ -1803,7 +1876,7 @@
       <c r="I11" s="16"/>
       <c r="J11" s="16"/>
     </row>
-    <row r="12" spans="1:10" ht="45.75">
+    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="16"/>
       <c r="B12" s="17">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
@@ -1824,7 +1897,7 @@
       <c r="I12" s="16"/>
       <c r="J12" s="16"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
       <c r="B13" s="17">
         <f t="shared" si="0"/>
@@ -1839,7 +1912,7 @@
       <c r="I13" s="16"/>
       <c r="J13" s="16"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="16"/>
       <c r="B14" s="17">
         <f t="shared" si="0"/>
@@ -1854,7 +1927,7 @@
       <c r="I14" s="16"/>
       <c r="J14" s="16"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="17">
         <f t="shared" si="0"/>
@@ -1869,7 +1942,7 @@
       <c r="I15" s="16"/>
       <c r="J15" s="16"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="16"/>
       <c r="B16" s="17">
         <f t="shared" si="0"/>
@@ -1884,7 +1957,7 @@
       <c r="I16" s="16"/>
       <c r="J16" s="16"/>
     </row>
-    <row r="17" spans="2:5">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="17">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1893,7 +1966,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="17">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1902,7 +1975,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="17">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1911,7 +1984,7 @@
       <c r="D19" s="1"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="17">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1920,7 +1993,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="17">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1929,7 +2002,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="17">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1938,7 +2011,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="17">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1947,7 +2020,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="17">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1956,7 +2029,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1965,7 +2038,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="17">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1974,7 +2047,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="17">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1983,7 +2056,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="2:5">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="17">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1992,7 +2065,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="2:5">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="17">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2001,7 +2074,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="2:5">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="17">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2010,13 +2083,13 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="2:5">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="16"/>
       <c r="C31" s="16"/>
       <c r="D31" s="16"/>
       <c r="E31" s="16"/>
     </row>
-    <row r="32" spans="2:5">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="16"/>
       <c r="C32" s="10" t="s">
         <v>18</v>
@@ -2049,7 +2122,7 @@
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="5"/>
     <col min="2" max="2" width="12.28515625" style="5" customWidth="1"/>
@@ -2062,7 +2135,7 @@
     <col min="10" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -2078,7 +2151,7 @@
       <c r="I1" s="20"/>
       <c r="J1" s="20"/>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="16"/>
       <c r="B2" s="21" t="s">
         <v>63</v>
@@ -2096,7 +2169,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="16"/>
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
@@ -2110,7 +2183,7 @@
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="16"/>
       <c r="B4" s="16"/>
       <c r="C4" s="14" t="s">
@@ -2126,7 +2199,7 @@
       <c r="I4" s="17"/>
       <c r="J4" s="17"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="B5" s="16"/>
       <c r="C5" s="8" t="s">
@@ -2142,7 +2215,7 @@
       <c r="I5" s="17"/>
       <c r="J5" s="17"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8" t="s">
@@ -2156,7 +2229,7 @@
       <c r="I6" s="16"/>
       <c r="J6" s="16"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
       <c r="B9" s="9" t="s">
         <v>14</v>
@@ -2178,7 +2251,7 @@
       <c r="I9" s="16"/>
       <c r="J9" s="16"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="16"/>
       <c r="B10" s="17">
         <v>1</v>
@@ -2192,7 +2265,7 @@
       <c r="I10" s="16"/>
       <c r="J10" s="16"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
       <c r="B11" s="17">
         <f>B10+1</f>
@@ -2207,7 +2280,7 @@
       <c r="I11" s="16"/>
       <c r="J11" s="16"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="16"/>
       <c r="B12" s="17">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
@@ -2222,7 +2295,7 @@
       <c r="I12" s="16"/>
       <c r="J12" s="16"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
       <c r="B13" s="17">
         <f t="shared" si="0"/>
@@ -2237,7 +2310,7 @@
       <c r="I13" s="16"/>
       <c r="J13" s="16"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="16"/>
       <c r="B14" s="17">
         <f t="shared" si="0"/>
@@ -2252,7 +2325,7 @@
       <c r="I14" s="16"/>
       <c r="J14" s="16"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="17">
         <f t="shared" si="0"/>
@@ -2267,7 +2340,7 @@
       <c r="I15" s="16"/>
       <c r="J15" s="16"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="16"/>
       <c r="B16" s="17">
         <f t="shared" si="0"/>
@@ -2282,7 +2355,7 @@
       <c r="I16" s="16"/>
       <c r="J16" s="16"/>
     </row>
-    <row r="17" spans="2:6">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="17">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2292,7 +2365,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="17">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2302,7 +2375,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="17">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2312,7 +2385,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="17">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2322,7 +2395,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="17">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2332,7 +2405,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="17">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2342,7 +2415,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="17">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2352,7 +2425,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="17">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2362,7 +2435,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2372,7 +2445,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:6">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="17">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2382,7 +2455,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="2:6">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="17">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2392,7 +2465,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="2:6">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="17">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2402,7 +2475,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="2:6">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="17">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2412,7 +2485,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="2:6">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="17">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2422,14 +2495,14 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="2:6">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="16"/>
       <c r="C31" s="16"/>
       <c r="D31" s="16"/>
       <c r="E31" s="16"/>
       <c r="F31" s="16"/>
     </row>
-    <row r="32" spans="2:6">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="16"/>
       <c r="C32" s="32" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
added code tool based code analysis
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="84">
   <si>
     <t xml:space="preserve">do not print this form</t>
   </si>
@@ -43,6 +43,9 @@
     <t xml:space="preserve">Student 1:</t>
   </si>
   <si>
+    <t xml:space="preserve">Haraseniuc Laura</t>
+  </si>
+  <si>
     <t xml:space="preserve">Document  Title:</t>
   </si>
   <si>
@@ -52,6 +55,9 @@
     <t xml:space="preserve">Student 2:</t>
   </si>
   <si>
+    <t xml:space="preserve">Berindean Razvan</t>
+  </si>
+  <si>
     <t xml:space="preserve">Author Name:</t>
   </si>
   <si>
@@ -61,6 +67,9 @@
     <t xml:space="preserve">Student 3:</t>
   </si>
   <si>
+    <t xml:space="preserve">Baluta Lucian</t>
+  </si>
+  <si>
     <t xml:space="preserve">Reviewer Name:</t>
   </si>
   <si>
@@ -85,22 +94,13 @@
     <t xml:space="preserve">Review Form. Architectural Design Defects</t>
   </si>
   <si>
-    <t xml:space="preserve">Haraseniuc Laura</t>
-  </si>
-  <si>
     <t xml:space="preserve">Architectural Design Document</t>
   </si>
   <si>
-    <t xml:space="preserve">Berindean Razvan</t>
-  </si>
-  <si>
     <t xml:space="preserve">Author Name: </t>
   </si>
   <si>
     <t xml:space="preserve">Georgescu Anca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Baluta Lucian</t>
   </si>
   <si>
     <t xml:space="preserve">A01</t>
@@ -654,8 +654,8 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -663,9 +663,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="16.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="41.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="41.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="1" width="8.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="20.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="8.86"/>
   </cols>
@@ -696,68 +696,80 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="6" t="n">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E4" s="8"/>
       <c r="H4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>9</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="6" t="n">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="7" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E5" s="9"/>
       <c r="H5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
+        <v>13</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="6" t="n">
+        <v>231</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="10"/>
       <c r="C6" s="11" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="13" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -905,7 +917,7 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="18" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D27" s="19"/>
       <c r="E27" s="15"/>
@@ -937,8 +949,8 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -946,7 +958,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="16.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="41.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="41.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="1" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="22.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="1" width="8.86"/>
@@ -965,7 +977,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -983,7 +995,7 @@
         <v>5</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="J3" s="6" t="n">
         <v>233</v>
@@ -991,17 +1003,17 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="20" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E4" s="21"/>
       <c r="H4" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="J4" s="6" t="n">
         <v>231</v>
@@ -1009,17 +1021,17 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="20" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E5" s="22"/>
       <c r="H5" s="6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="J5" s="6" t="n">
         <v>231</v>
@@ -1028,16 +1040,16 @@
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="10"/>
       <c r="C6" s="11" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="E6" s="12"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D7" s="23" t="n">
         <v>45361</v>
@@ -1046,16 +1058,16 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="13" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1288,7 +1300,7 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="18" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D28" s="19"/>
       <c r="E28" s="15"/>
@@ -1320,8 +1332,8 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1330,7 +1342,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="41.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="41.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="1" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="26.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="1" width="8.86"/>
@@ -1362,68 +1374,80 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="6" t="n">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="24" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D4" s="25" t="s">
         <v>61</v>
       </c>
       <c r="E4" s="25"/>
       <c r="H4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>9</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="6" t="n">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="24" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D5" s="26" t="s">
         <v>62</v>
       </c>
       <c r="E5" s="26"/>
       <c r="H5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
+        <v>13</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="6" t="n">
+        <v>231</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="10"/>
       <c r="C6" s="11" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="13" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1652,7 +1676,7 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="18" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D32" s="19"/>
       <c r="E32" s="15"/>
@@ -1685,7 +1709,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
+      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1727,48 +1751,60 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="6" t="n">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="24" t="s">
         <v>78</v>
       </c>
       <c r="D4" s="25"/>
       <c r="E4" s="25"/>
       <c r="H4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>9</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="6" t="n">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="11" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
       <c r="H5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
+        <v>13</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="6" t="n">
+        <v>231</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="10"/>
       <c r="C6" s="11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="13" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>79</v>

</xml_diff>